<commit_message>
Fixed inspection plan logic and column mapping
</commit_message>
<xml_diff>
--- a/outputs/10_output.xlsx
+++ b/outputs/10_output.xlsx
@@ -1,12 +1,12 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="191029" fullCalcOnLoad="1"/>
@@ -353,7 +353,7 @@
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<wsDr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+<wsDr xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
   <oneCellAnchor>
     <from>
       <col>11</col>
@@ -368,21 +368,21 @@
         <cNvPicPr preferRelativeResize="0"/>
       </nvPicPr>
       <blipFill>
-        <a:blip cstate="print" r:embed="rId1"/>
-        <a:stretch>
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId1"/>
+        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:fillRect/>
         </a:stretch>
       </blipFill>
       <spPr>
-        <a:xfrm>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:off x="7513320" y="137160"/>
           <a:ext cx="2095500" cy="523875"/>
         </a:xfrm>
-        <a:prstGeom prst="rect">
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
           <avLst/>
         </a:prstGeom>
-        <a:noFill/>
-        <a:ln>
+        <a:noFill xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
+        <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:prstDash val="solid"/>
         </a:ln>
       </spPr>
@@ -693,7 +693,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:O21"/>
+  <dimension ref="A1:O53"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A8" sqref="A8"/>
@@ -879,18 +879,18 @@
       </c>
       <c r="C8" s="29" t="inlineStr">
         <is>
-          <t>MLK_PMT_10102_-_V-002</t>
+          <t>MLK_PMT_10104_-_V-004</t>
         </is>
       </c>
       <c r="D8" s="29" t="inlineStr"/>
       <c r="E8" t="inlineStr">
         <is>
-          <t>PLATE 157x600x5mm SHELL TO BE ROLLED</t>
+          <t>Shell Plate</t>
         </is>
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>DMSO</t>
+          <t>HOT WATER</t>
         </is>
       </c>
       <c r="H8" t="inlineStr">
@@ -900,12 +900,12 @@
       </c>
       <c r="I8" t="inlineStr">
         <is>
-          <t>SA 240 M</t>
+          <t>ASTM A240</t>
         </is>
       </c>
       <c r="J8" t="inlineStr">
         <is>
-          <t>316L</t>
+          <t>304L</t>
         </is>
       </c>
       <c r="K8" t="inlineStr">
@@ -915,34 +915,34 @@
       </c>
       <c r="L8" t="inlineStr">
         <is>
-          <t>100 °C</t>
+          <t>120 °C</t>
         </is>
       </c>
       <c r="M8" t="inlineStr">
         <is>
-          <t>1.1 BarG</t>
+          <t>4 Bar</t>
         </is>
       </c>
       <c r="N8" t="inlineStr">
         <is>
-          <t>100 °C</t>
+          <t>90 °C</t>
         </is>
       </c>
       <c r="O8" t="inlineStr">
         <is>
-          <t>1.0 BarG</t>
+          <t>1 Bar</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="E9" t="inlineStr">
         <is>
-          <t>DISH HEAD 8 THK TO BE FORMED T.O 2:1 TYPE</t>
+          <t>2:1 Ellipsoidal Head</t>
         </is>
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>DMSO</t>
+          <t>HOT WATER</t>
         </is>
       </c>
       <c r="H9" t="inlineStr">
@@ -952,12 +952,12 @@
       </c>
       <c r="I9" t="inlineStr">
         <is>
-          <t>SA 240 M</t>
+          <t>ASTM A240</t>
         </is>
       </c>
       <c r="J9" t="inlineStr">
         <is>
-          <t>316L</t>
+          <t>304L</t>
         </is>
       </c>
       <c r="K9" t="inlineStr">
@@ -967,34 +967,34 @@
       </c>
       <c r="L9" t="inlineStr">
         <is>
-          <t>100 °C</t>
+          <t>120 °C</t>
         </is>
       </c>
       <c r="M9" t="inlineStr">
         <is>
-          <t>1.1 BarG</t>
+          <t>4 Bar</t>
         </is>
       </c>
       <c r="N9" t="inlineStr">
         <is>
-          <t>100 °C</t>
+          <t>90 °C</t>
         </is>
       </c>
       <c r="O9" t="inlineStr">
         <is>
-          <t>1.0 BarG</t>
+          <t>1 Bar</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="E10" t="inlineStr">
         <is>
-          <t>SEAMLESS PIPE DN50 x 87 SCH 40s</t>
+          <t>Lifting Lug</t>
         </is>
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>DMSO</t>
+          <t>HOT WATER</t>
         </is>
       </c>
       <c r="H10" t="inlineStr">
@@ -1004,12 +1004,12 @@
       </c>
       <c r="I10" t="inlineStr">
         <is>
-          <t>SA 312 M TP</t>
+          <t>ASTM A240</t>
         </is>
       </c>
       <c r="J10" t="inlineStr">
         <is>
-          <t>316L</t>
+          <t>304L</t>
         </is>
       </c>
       <c r="K10" t="inlineStr">
@@ -1019,34 +1019,34 @@
       </c>
       <c r="L10" t="inlineStr">
         <is>
-          <t>100 °C</t>
+          <t>120 °C</t>
         </is>
       </c>
       <c r="M10" t="inlineStr">
         <is>
-          <t>1.1 BarG</t>
+          <t>4 Bar</t>
         </is>
       </c>
       <c r="N10" t="inlineStr">
         <is>
-          <t>100 °C</t>
+          <t>90 °C</t>
         </is>
       </c>
       <c r="O10" t="inlineStr">
         <is>
-          <t>1.0 BarG</t>
+          <t>1 Bar</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="E11" t="inlineStr">
         <is>
-          <t>SEAMLESS PIPE DN25 x 100 SCH 40s</t>
+          <t>Lifting Lug</t>
         </is>
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>DMSO</t>
+          <t>HOT WATER</t>
         </is>
       </c>
       <c r="H11" t="inlineStr">
@@ -1056,12 +1056,12 @@
       </c>
       <c r="I11" t="inlineStr">
         <is>
-          <t>SA 312 M TP</t>
+          <t>ASTM A240</t>
         </is>
       </c>
       <c r="J11" t="inlineStr">
         <is>
-          <t>316L</t>
+          <t>304L</t>
         </is>
       </c>
       <c r="K11" t="inlineStr">
@@ -1071,34 +1071,34 @@
       </c>
       <c r="L11" t="inlineStr">
         <is>
-          <t>100 °C</t>
+          <t>120 °C</t>
         </is>
       </c>
       <c r="M11" t="inlineStr">
         <is>
-          <t>1.1 BarG</t>
+          <t>4 Bar</t>
         </is>
       </c>
       <c r="N11" t="inlineStr">
         <is>
-          <t>100 °C</t>
+          <t>90 °C</t>
         </is>
       </c>
       <c r="O11" t="inlineStr">
         <is>
-          <t>1.0 BarG</t>
+          <t>1 Bar</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="E12" t="inlineStr">
         <is>
-          <t>SEAMLESS PIPE DN50 x 112 SCH 40s</t>
+          <t>Saddle Plate</t>
         </is>
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>DMSO</t>
+          <t>HOT WATER</t>
         </is>
       </c>
       <c r="H12" t="inlineStr">
@@ -1108,12 +1108,12 @@
       </c>
       <c r="I12" t="inlineStr">
         <is>
-          <t>SA 312 M TP</t>
+          <t>ASTM A240</t>
         </is>
       </c>
       <c r="J12" t="inlineStr">
         <is>
-          <t>316L</t>
+          <t>304L</t>
         </is>
       </c>
       <c r="K12" t="inlineStr">
@@ -1123,34 +1123,34 @@
       </c>
       <c r="L12" t="inlineStr">
         <is>
-          <t>100 °C</t>
+          <t>120 °C</t>
         </is>
       </c>
       <c r="M12" t="inlineStr">
         <is>
-          <t>1.1 BarG</t>
+          <t>4 Bar</t>
         </is>
       </c>
       <c r="N12" t="inlineStr">
         <is>
-          <t>100 °C</t>
+          <t>90 °C</t>
         </is>
       </c>
       <c r="O12" t="inlineStr">
         <is>
-          <t>1.0 BarG</t>
+          <t>1 Bar</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="E13" t="inlineStr">
         <is>
-          <t>FLANGE DN50 CLASS 150 WNRF SCH 40s</t>
+          <t>Saddle Baseplate</t>
         </is>
       </c>
       <c r="G13" t="inlineStr">
         <is>
-          <t>DMSO</t>
+          <t>HOT WATER</t>
         </is>
       </c>
       <c r="H13" t="inlineStr">
@@ -1160,12 +1160,12 @@
       </c>
       <c r="I13" t="inlineStr">
         <is>
-          <t>SA 182 M</t>
+          <t>ASTM A240</t>
         </is>
       </c>
       <c r="J13" t="inlineStr">
         <is>
-          <t>F316L</t>
+          <t>304L</t>
         </is>
       </c>
       <c r="K13" t="inlineStr">
@@ -1175,34 +1175,34 @@
       </c>
       <c r="L13" t="inlineStr">
         <is>
-          <t>100 °C</t>
+          <t>120 °C</t>
         </is>
       </c>
       <c r="M13" t="inlineStr">
         <is>
-          <t>1.1 BarG</t>
+          <t>4 Bar</t>
         </is>
       </c>
       <c r="N13" t="inlineStr">
         <is>
-          <t>100 °C</t>
+          <t>90 °C</t>
         </is>
       </c>
       <c r="O13" t="inlineStr">
         <is>
-          <t>1.0 BarG</t>
+          <t>1 Bar</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="E14" t="inlineStr">
         <is>
-          <t>FLANGE DN25 CLASS 150 WNRF SCH 40s</t>
+          <t>Saddle Baseplate</t>
         </is>
       </c>
       <c r="G14" t="inlineStr">
         <is>
-          <t>DMSO</t>
+          <t>HOT WATER</t>
         </is>
       </c>
       <c r="H14" t="inlineStr">
@@ -1212,12 +1212,12 @@
       </c>
       <c r="I14" t="inlineStr">
         <is>
-          <t>SA 182 M</t>
+          <t>ASTM A240</t>
         </is>
       </c>
       <c r="J14" t="inlineStr">
         <is>
-          <t>F316L</t>
+          <t>304L</t>
         </is>
       </c>
       <c r="K14" t="inlineStr">
@@ -1227,34 +1227,34 @@
       </c>
       <c r="L14" t="inlineStr">
         <is>
-          <t>100 °C</t>
+          <t>120 °C</t>
         </is>
       </c>
       <c r="M14" t="inlineStr">
         <is>
-          <t>1.1 BarG</t>
+          <t>4 Bar</t>
         </is>
       </c>
       <c r="N14" t="inlineStr">
         <is>
-          <t>100 °C</t>
+          <t>90 °C</t>
         </is>
       </c>
       <c r="O14" t="inlineStr">
         <is>
-          <t>1.0 BarG</t>
+          <t>1 Bar</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="E15" t="inlineStr">
         <is>
-          <t>FLANGE DN50 CLASS 150 WNRF SCH 40s</t>
+          <t>Saddle Baseplate</t>
         </is>
       </c>
       <c r="G15" t="inlineStr">
         <is>
-          <t>DMSO</t>
+          <t>HOT WATER</t>
         </is>
       </c>
       <c r="H15" t="inlineStr">
@@ -1264,12 +1264,12 @@
       </c>
       <c r="I15" t="inlineStr">
         <is>
-          <t>SA 182 M</t>
+          <t>ASTM A240</t>
         </is>
       </c>
       <c r="J15" t="inlineStr">
         <is>
-          <t>F316L</t>
+          <t>304L</t>
         </is>
       </c>
       <c r="K15" t="inlineStr">
@@ -1279,34 +1279,34 @@
       </c>
       <c r="L15" t="inlineStr">
         <is>
-          <t>100 °C</t>
+          <t>120 °C</t>
         </is>
       </c>
       <c r="M15" t="inlineStr">
         <is>
-          <t>1.1 BarG</t>
+          <t>4 Bar</t>
         </is>
       </c>
       <c r="N15" t="inlineStr">
         <is>
-          <t>100 °C</t>
+          <t>90 °C</t>
         </is>
       </c>
       <c r="O15" t="inlineStr">
         <is>
-          <t>1.0 BarG</t>
+          <t>1 Bar</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="E16" t="inlineStr">
         <is>
-          <t>BASE PLATE 150 x 150 x 5 THK</t>
+          <t>Flange</t>
         </is>
       </c>
       <c r="G16" t="inlineStr">
         <is>
-          <t>DMSO</t>
+          <t>HOT WATER</t>
         </is>
       </c>
       <c r="H16" t="inlineStr">
@@ -1316,12 +1316,12 @@
       </c>
       <c r="I16" t="inlineStr">
         <is>
-          <t>SA 240 M</t>
+          <t>ASTM A182</t>
         </is>
       </c>
       <c r="J16" t="inlineStr">
         <is>
-          <t>304</t>
+          <t>F304L</t>
         </is>
       </c>
       <c r="K16" t="inlineStr">
@@ -1331,34 +1331,34 @@
       </c>
       <c r="L16" t="inlineStr">
         <is>
-          <t>100 °C</t>
+          <t>120 °C</t>
         </is>
       </c>
       <c r="M16" t="inlineStr">
         <is>
-          <t>1.1 BarG</t>
+          <t>4 Bar</t>
         </is>
       </c>
       <c r="N16" t="inlineStr">
         <is>
-          <t>100 °C</t>
+          <t>90 °C</t>
         </is>
       </c>
       <c r="O16" t="inlineStr">
         <is>
-          <t>1.0 BarG</t>
+          <t>1 Bar</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="E17" t="inlineStr">
         <is>
-          <t>LIFTING LUG PLATE 190 x 80 x 6 THK</t>
+          <t>Flange</t>
         </is>
       </c>
       <c r="G17" t="inlineStr">
         <is>
-          <t>DMSO</t>
+          <t>HOT WATER</t>
         </is>
       </c>
       <c r="H17" t="inlineStr">
@@ -1368,12 +1368,12 @@
       </c>
       <c r="I17" t="inlineStr">
         <is>
-          <t>SA 240 M</t>
+          <t>ASTM A182</t>
         </is>
       </c>
       <c r="J17" t="inlineStr">
         <is>
-          <t>316L</t>
+          <t>F304L</t>
         </is>
       </c>
       <c r="K17" t="inlineStr">
@@ -1383,34 +1383,34 @@
       </c>
       <c r="L17" t="inlineStr">
         <is>
-          <t>100 °C</t>
+          <t>120 °C</t>
         </is>
       </c>
       <c r="M17" t="inlineStr">
         <is>
-          <t>1.1 BarG</t>
+          <t>4 Bar</t>
         </is>
       </c>
       <c r="N17" t="inlineStr">
         <is>
-          <t>100 °C</t>
+          <t>90 °C</t>
         </is>
       </c>
       <c r="O17" t="inlineStr">
         <is>
-          <t>1.0 BarG</t>
+          <t>1 Bar</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="E18" t="inlineStr">
         <is>
-          <t>DOUBLER PLATE 120 x 150 x 12.7 THK</t>
+          <t>Neck</t>
         </is>
       </c>
       <c r="G18" t="inlineStr">
         <is>
-          <t>DMSO</t>
+          <t>HOT WATER</t>
         </is>
       </c>
       <c r="H18" t="inlineStr">
@@ -1420,12 +1420,12 @@
       </c>
       <c r="I18" t="inlineStr">
         <is>
-          <t>SA 240 M</t>
+          <t>ASTM A312</t>
         </is>
       </c>
       <c r="J18" t="inlineStr">
         <is>
-          <t>304</t>
+          <t>TP304L</t>
         </is>
       </c>
       <c r="K18" t="inlineStr">
@@ -1435,34 +1435,34 @@
       </c>
       <c r="L18" t="inlineStr">
         <is>
-          <t>100 °C</t>
+          <t>120 °C</t>
         </is>
       </c>
       <c r="M18" t="inlineStr">
         <is>
-          <t>1.1 BarG</t>
+          <t>4 Bar</t>
         </is>
       </c>
       <c r="N18" t="inlineStr">
         <is>
-          <t>100 °C</t>
+          <t>90 °C</t>
         </is>
       </c>
       <c r="O18" t="inlineStr">
         <is>
-          <t>1.0 BarG</t>
+          <t>1 Bar</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="E19" t="inlineStr">
         <is>
-          <t>EQUAL ANGLE BAR 3" x 3" x 1/4" THK</t>
+          <t>Neck</t>
         </is>
       </c>
       <c r="G19" t="inlineStr">
         <is>
-          <t>DMSO</t>
+          <t>HOT WATER</t>
         </is>
       </c>
       <c r="H19" t="inlineStr">
@@ -1472,12 +1472,12 @@
       </c>
       <c r="I19" t="inlineStr">
         <is>
-          <t>SA 240 M</t>
+          <t>ASTM A312</t>
         </is>
       </c>
       <c r="J19" t="inlineStr">
         <is>
-          <t>304</t>
+          <t>TP304L</t>
         </is>
       </c>
       <c r="K19" t="inlineStr">
@@ -1487,34 +1487,34 @@
       </c>
       <c r="L19" t="inlineStr">
         <is>
-          <t>100 °C</t>
+          <t>120 °C</t>
         </is>
       </c>
       <c r="M19" t="inlineStr">
         <is>
-          <t>1.1 BarG</t>
+          <t>4 Bar</t>
         </is>
       </c>
       <c r="N19" t="inlineStr">
         <is>
-          <t>100 °C</t>
+          <t>90 °C</t>
         </is>
       </c>
       <c r="O19" t="inlineStr">
         <is>
-          <t>1.0 BarG</t>
+          <t>1 Bar</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="E20" t="inlineStr">
         <is>
-          <t>EARTHING LUG</t>
+          <t>Flange</t>
         </is>
       </c>
       <c r="G20" t="inlineStr">
         <is>
-          <t>DMSO</t>
+          <t>HOT WATER</t>
         </is>
       </c>
       <c r="H20" t="inlineStr">
@@ -1524,12 +1524,12 @@
       </c>
       <c r="I20" t="inlineStr">
         <is>
-          <t>SA 240 M</t>
+          <t>ASTM A182</t>
         </is>
       </c>
       <c r="J20" t="inlineStr">
         <is>
-          <t>304</t>
+          <t>F304L</t>
         </is>
       </c>
       <c r="K20" t="inlineStr">
@@ -1539,90 +1539,1754 @@
       </c>
       <c r="L20" t="inlineStr">
         <is>
-          <t>100 °C</t>
+          <t>120 °C</t>
         </is>
       </c>
       <c r="M20" t="inlineStr">
         <is>
-          <t>1.1 BarG</t>
+          <t>4 Bar</t>
         </is>
       </c>
       <c r="N20" t="inlineStr">
         <is>
-          <t>100 °C</t>
+          <t>90 °C</t>
         </is>
       </c>
       <c r="O20" t="inlineStr">
         <is>
-          <t>1.0 BarG</t>
+          <t>1 Bar</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="E21" t="inlineStr">
         <is>
-          <t>NAMEPLATE</t>
+          <t>Flange</t>
         </is>
       </c>
       <c r="G21" t="inlineStr">
         <is>
-          <t>DMSO</t>
+          <t>HOT WATER</t>
         </is>
       </c>
       <c r="H21" t="inlineStr">
         <is>
+          <t>Stainless Steel</t>
+        </is>
+      </c>
+      <c r="I21" t="inlineStr">
+        <is>
+          <t>ASTM A182</t>
+        </is>
+      </c>
+      <c r="J21" t="inlineStr">
+        <is>
+          <t>F304L</t>
+        </is>
+      </c>
+      <c r="K21" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="L21" t="inlineStr">
+        <is>
+          <t>120 °C</t>
+        </is>
+      </c>
+      <c r="M21" t="inlineStr">
+        <is>
+          <t>4 Bar</t>
+        </is>
+      </c>
+      <c r="N21" t="inlineStr">
+        <is>
+          <t>90 °C</t>
+        </is>
+      </c>
+      <c r="O21" t="inlineStr">
+        <is>
+          <t>1 Bar</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>Neck</t>
+        </is>
+      </c>
+      <c r="G22" t="inlineStr">
+        <is>
+          <t>HOT WATER</t>
+        </is>
+      </c>
+      <c r="H22" t="inlineStr">
+        <is>
+          <t>Stainless Steel</t>
+        </is>
+      </c>
+      <c r="I22" t="inlineStr">
+        <is>
+          <t>ASTM A312</t>
+        </is>
+      </c>
+      <c r="J22" t="inlineStr">
+        <is>
+          <t>TP304L</t>
+        </is>
+      </c>
+      <c r="K22" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="L22" t="inlineStr">
+        <is>
+          <t>120 °C</t>
+        </is>
+      </c>
+      <c r="M22" t="inlineStr">
+        <is>
+          <t>4 Bar</t>
+        </is>
+      </c>
+      <c r="N22" t="inlineStr">
+        <is>
+          <t>90 °C</t>
+        </is>
+      </c>
+      <c r="O22" t="inlineStr">
+        <is>
+          <t>1 Bar</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="E23" t="inlineStr">
+        <is>
+          <t>Flange</t>
+        </is>
+      </c>
+      <c r="G23" t="inlineStr">
+        <is>
+          <t>HOT WATER</t>
+        </is>
+      </c>
+      <c r="H23" t="inlineStr">
+        <is>
+          <t>Stainless Steel</t>
+        </is>
+      </c>
+      <c r="I23" t="inlineStr">
+        <is>
+          <t>ASTM A182</t>
+        </is>
+      </c>
+      <c r="J23" t="inlineStr">
+        <is>
+          <t>F304L</t>
+        </is>
+      </c>
+      <c r="K23" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="L23" t="inlineStr">
+        <is>
+          <t>120 °C</t>
+        </is>
+      </c>
+      <c r="M23" t="inlineStr">
+        <is>
+          <t>4 Bar</t>
+        </is>
+      </c>
+      <c r="N23" t="inlineStr">
+        <is>
+          <t>90 °C</t>
+        </is>
+      </c>
+      <c r="O23" t="inlineStr">
+        <is>
+          <t>1 Bar</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="E24" t="inlineStr">
+        <is>
+          <t>Flange</t>
+        </is>
+      </c>
+      <c r="G24" t="inlineStr">
+        <is>
+          <t>HOT WATER</t>
+        </is>
+      </c>
+      <c r="H24" t="inlineStr">
+        <is>
+          <t>Stainless Steel</t>
+        </is>
+      </c>
+      <c r="I24" t="inlineStr">
+        <is>
+          <t>ASTM A182</t>
+        </is>
+      </c>
+      <c r="J24" t="inlineStr">
+        <is>
+          <t>F304L</t>
+        </is>
+      </c>
+      <c r="K24" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="L24" t="inlineStr">
+        <is>
+          <t>120 °C</t>
+        </is>
+      </c>
+      <c r="M24" t="inlineStr">
+        <is>
+          <t>4 Bar</t>
+        </is>
+      </c>
+      <c r="N24" t="inlineStr">
+        <is>
+          <t>90 °C</t>
+        </is>
+      </c>
+      <c r="O24" t="inlineStr">
+        <is>
+          <t>1 Bar</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="E25" t="inlineStr">
+        <is>
+          <t>Neck</t>
+        </is>
+      </c>
+      <c r="G25" t="inlineStr">
+        <is>
+          <t>HOT WATER</t>
+        </is>
+      </c>
+      <c r="H25" t="inlineStr">
+        <is>
+          <t>Stainless Steel</t>
+        </is>
+      </c>
+      <c r="I25" t="inlineStr">
+        <is>
+          <t>ASTM A312</t>
+        </is>
+      </c>
+      <c r="J25" t="inlineStr">
+        <is>
+          <t>TP304L</t>
+        </is>
+      </c>
+      <c r="K25" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="L25" t="inlineStr">
+        <is>
+          <t>120 °C</t>
+        </is>
+      </c>
+      <c r="M25" t="inlineStr">
+        <is>
+          <t>4 Bar</t>
+        </is>
+      </c>
+      <c r="N25" t="inlineStr">
+        <is>
+          <t>90 °C</t>
+        </is>
+      </c>
+      <c r="O25" t="inlineStr">
+        <is>
+          <t>1 Bar</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="E26" t="inlineStr">
+        <is>
+          <t>Neck</t>
+        </is>
+      </c>
+      <c r="G26" t="inlineStr">
+        <is>
+          <t>HOT WATER</t>
+        </is>
+      </c>
+      <c r="H26" t="inlineStr">
+        <is>
+          <t>Stainless Steel</t>
+        </is>
+      </c>
+      <c r="I26" t="inlineStr">
+        <is>
+          <t>ASTM A312</t>
+        </is>
+      </c>
+      <c r="J26" t="inlineStr">
+        <is>
+          <t>TP304L</t>
+        </is>
+      </c>
+      <c r="K26" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="L26" t="inlineStr">
+        <is>
+          <t>120 °C</t>
+        </is>
+      </c>
+      <c r="M26" t="inlineStr">
+        <is>
+          <t>4 Bar</t>
+        </is>
+      </c>
+      <c r="N26" t="inlineStr">
+        <is>
+          <t>90 °C</t>
+        </is>
+      </c>
+      <c r="O26" t="inlineStr">
+        <is>
+          <t>1 Bar</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="E27" t="inlineStr">
+        <is>
+          <t>Flange</t>
+        </is>
+      </c>
+      <c r="G27" t="inlineStr">
+        <is>
+          <t>HOT WATER</t>
+        </is>
+      </c>
+      <c r="H27" t="inlineStr">
+        <is>
+          <t>Stainless Steel</t>
+        </is>
+      </c>
+      <c r="I27" t="inlineStr">
+        <is>
+          <t>ASTM A182</t>
+        </is>
+      </c>
+      <c r="J27" t="inlineStr">
+        <is>
+          <t>F304L</t>
+        </is>
+      </c>
+      <c r="K27" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="L27" t="inlineStr">
+        <is>
+          <t>120 °C</t>
+        </is>
+      </c>
+      <c r="M27" t="inlineStr">
+        <is>
+          <t>4 Bar</t>
+        </is>
+      </c>
+      <c r="N27" t="inlineStr">
+        <is>
+          <t>90 °C</t>
+        </is>
+      </c>
+      <c r="O27" t="inlineStr">
+        <is>
+          <t>1 Bar</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="E28" t="inlineStr">
+        <is>
+          <t>Flange</t>
+        </is>
+      </c>
+      <c r="G28" t="inlineStr">
+        <is>
+          <t>HOT WATER</t>
+        </is>
+      </c>
+      <c r="H28" t="inlineStr">
+        <is>
+          <t>Stainless Steel</t>
+        </is>
+      </c>
+      <c r="I28" t="inlineStr">
+        <is>
+          <t>ASTM A182</t>
+        </is>
+      </c>
+      <c r="J28" t="inlineStr">
+        <is>
+          <t>F304L</t>
+        </is>
+      </c>
+      <c r="K28" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="L28" t="inlineStr">
+        <is>
+          <t>120 °C</t>
+        </is>
+      </c>
+      <c r="M28" t="inlineStr">
+        <is>
+          <t>4 Bar</t>
+        </is>
+      </c>
+      <c r="N28" t="inlineStr">
+        <is>
+          <t>90 °C</t>
+        </is>
+      </c>
+      <c r="O28" t="inlineStr">
+        <is>
+          <t>1 Bar</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="E29" t="inlineStr">
+        <is>
+          <t>Neck</t>
+        </is>
+      </c>
+      <c r="G29" t="inlineStr">
+        <is>
+          <t>HOT WATER</t>
+        </is>
+      </c>
+      <c r="H29" t="inlineStr">
+        <is>
+          <t>Stainless Steel</t>
+        </is>
+      </c>
+      <c r="I29" t="inlineStr">
+        <is>
+          <t>ASTM A312</t>
+        </is>
+      </c>
+      <c r="J29" t="inlineStr">
+        <is>
+          <t>TP304L</t>
+        </is>
+      </c>
+      <c r="K29" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="L29" t="inlineStr">
+        <is>
+          <t>120 °C</t>
+        </is>
+      </c>
+      <c r="M29" t="inlineStr">
+        <is>
+          <t>4 Bar</t>
+        </is>
+      </c>
+      <c r="N29" t="inlineStr">
+        <is>
+          <t>90 °C</t>
+        </is>
+      </c>
+      <c r="O29" t="inlineStr">
+        <is>
+          <t>1 Bar</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="E30" t="inlineStr">
+        <is>
+          <t>Neck</t>
+        </is>
+      </c>
+      <c r="G30" t="inlineStr">
+        <is>
+          <t>HOT WATER</t>
+        </is>
+      </c>
+      <c r="H30" t="inlineStr">
+        <is>
+          <t>Stainless Steel</t>
+        </is>
+      </c>
+      <c r="I30" t="inlineStr">
+        <is>
+          <t>ASTM A312</t>
+        </is>
+      </c>
+      <c r="J30" t="inlineStr">
+        <is>
+          <t>TP304L</t>
+        </is>
+      </c>
+      <c r="K30" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="L30" t="inlineStr">
+        <is>
+          <t>120 °C</t>
+        </is>
+      </c>
+      <c r="M30" t="inlineStr">
+        <is>
+          <t>4 Bar</t>
+        </is>
+      </c>
+      <c r="N30" t="inlineStr">
+        <is>
+          <t>90 °C</t>
+        </is>
+      </c>
+      <c r="O30" t="inlineStr">
+        <is>
+          <t>1 Bar</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="E31" t="inlineStr">
+        <is>
+          <t>Blind Flange</t>
+        </is>
+      </c>
+      <c r="G31" t="inlineStr">
+        <is>
+          <t>HOT WATER</t>
+        </is>
+      </c>
+      <c r="H31" t="inlineStr">
+        <is>
+          <t>Stainless Steel</t>
+        </is>
+      </c>
+      <c r="I31" t="inlineStr">
+        <is>
+          <t>ASTM A182</t>
+        </is>
+      </c>
+      <c r="J31" t="inlineStr">
+        <is>
+          <t>F304L</t>
+        </is>
+      </c>
+      <c r="K31" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="L31" t="inlineStr">
+        <is>
+          <t>120 °C</t>
+        </is>
+      </c>
+      <c r="M31" t="inlineStr">
+        <is>
+          <t>4 Bar</t>
+        </is>
+      </c>
+      <c r="N31" t="inlineStr">
+        <is>
+          <t>90 °C</t>
+        </is>
+      </c>
+      <c r="O31" t="inlineStr">
+        <is>
+          <t>1 Bar</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="E32" t="inlineStr">
+        <is>
+          <t>Spiral Wound Gasket</t>
+        </is>
+      </c>
+      <c r="G32" t="inlineStr">
+        <is>
+          <t>HOT WATER</t>
+        </is>
+      </c>
+      <c r="H32" t="inlineStr">
+        <is>
           <t>Not Found</t>
         </is>
       </c>
-      <c r="I21" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="K21" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-      <c r="L21" t="inlineStr">
-        <is>
-          <t>100 °C</t>
-        </is>
-      </c>
-      <c r="M21" t="inlineStr">
-        <is>
-          <t>1.1 BarG</t>
-        </is>
-      </c>
-      <c r="N21" t="inlineStr">
-        <is>
-          <t>100 °C</t>
-        </is>
-      </c>
-      <c r="O21" t="inlineStr">
-        <is>
-          <t>1.0 BarG</t>
+      <c r="I32" t="inlineStr">
+        <is>
+          <t>ASME B16.20</t>
+        </is>
+      </c>
+      <c r="K32" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="L32" t="inlineStr">
+        <is>
+          <t>120 °C</t>
+        </is>
+      </c>
+      <c r="M32" t="inlineStr">
+        <is>
+          <t>4 Bar</t>
+        </is>
+      </c>
+      <c r="N32" t="inlineStr">
+        <is>
+          <t>90 °C</t>
+        </is>
+      </c>
+      <c r="O32" t="inlineStr">
+        <is>
+          <t>1 Bar</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="E33" t="inlineStr">
+        <is>
+          <t>Flange</t>
+        </is>
+      </c>
+      <c r="G33" t="inlineStr">
+        <is>
+          <t>HOT WATER</t>
+        </is>
+      </c>
+      <c r="H33" t="inlineStr">
+        <is>
+          <t>Stainless Steel</t>
+        </is>
+      </c>
+      <c r="I33" t="inlineStr">
+        <is>
+          <t>ASTM A182</t>
+        </is>
+      </c>
+      <c r="J33" t="inlineStr">
+        <is>
+          <t>F304L</t>
+        </is>
+      </c>
+      <c r="K33" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="L33" t="inlineStr">
+        <is>
+          <t>120 °C</t>
+        </is>
+      </c>
+      <c r="M33" t="inlineStr">
+        <is>
+          <t>4 Bar</t>
+        </is>
+      </c>
+      <c r="N33" t="inlineStr">
+        <is>
+          <t>90 °C</t>
+        </is>
+      </c>
+      <c r="O33" t="inlineStr">
+        <is>
+          <t>1 Bar</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="E34" t="inlineStr">
+        <is>
+          <t>Neck</t>
+        </is>
+      </c>
+      <c r="G34" t="inlineStr">
+        <is>
+          <t>HOT WATER</t>
+        </is>
+      </c>
+      <c r="H34" t="inlineStr">
+        <is>
+          <t>Stainless Steel</t>
+        </is>
+      </c>
+      <c r="I34" t="inlineStr">
+        <is>
+          <t>ASTM A312</t>
+        </is>
+      </c>
+      <c r="J34" t="inlineStr">
+        <is>
+          <t>TP304L</t>
+        </is>
+      </c>
+      <c r="K34" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="L34" t="inlineStr">
+        <is>
+          <t>120 °C</t>
+        </is>
+      </c>
+      <c r="M34" t="inlineStr">
+        <is>
+          <t>4 Bar</t>
+        </is>
+      </c>
+      <c r="N34" t="inlineStr">
+        <is>
+          <t>90 °C</t>
+        </is>
+      </c>
+      <c r="O34" t="inlineStr">
+        <is>
+          <t>1 Bar</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="E35" t="inlineStr">
+        <is>
+          <t>Stud Bolt</t>
+        </is>
+      </c>
+      <c r="G35" t="inlineStr">
+        <is>
+          <t>HOT WATER</t>
+        </is>
+      </c>
+      <c r="H35" t="inlineStr">
+        <is>
+          <t>Stainless Steel Bolting</t>
+        </is>
+      </c>
+      <c r="I35" t="inlineStr">
+        <is>
+          <t>ASTM A193</t>
+        </is>
+      </c>
+      <c r="J35" t="inlineStr">
+        <is>
+          <t>B8M</t>
+        </is>
+      </c>
+      <c r="K35" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="L35" t="inlineStr">
+        <is>
+          <t>120 °C</t>
+        </is>
+      </c>
+      <c r="M35" t="inlineStr">
+        <is>
+          <t>4 Bar</t>
+        </is>
+      </c>
+      <c r="N35" t="inlineStr">
+        <is>
+          <t>90 °C</t>
+        </is>
+      </c>
+      <c r="O35" t="inlineStr">
+        <is>
+          <t>1 Bar</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="E36" t="inlineStr">
+        <is>
+          <t>Nuts &amp; Washer</t>
+        </is>
+      </c>
+      <c r="G36" t="inlineStr">
+        <is>
+          <t>HOT WATER</t>
+        </is>
+      </c>
+      <c r="H36" t="inlineStr">
+        <is>
+          <t>Heavy Hex Nuts</t>
+        </is>
+      </c>
+      <c r="I36" t="inlineStr">
+        <is>
+          <t>ASTM A194</t>
+        </is>
+      </c>
+      <c r="J36" t="inlineStr">
+        <is>
+          <t>2H</t>
+        </is>
+      </c>
+      <c r="K36" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="L36" t="inlineStr">
+        <is>
+          <t>120 °C</t>
+        </is>
+      </c>
+      <c r="M36" t="inlineStr">
+        <is>
+          <t>4 Bar</t>
+        </is>
+      </c>
+      <c r="N36" t="inlineStr">
+        <is>
+          <t>90 °C</t>
+        </is>
+      </c>
+      <c r="O36" t="inlineStr">
+        <is>
+          <t>1 Bar</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="E37" t="inlineStr">
+        <is>
+          <t>Bracket 1</t>
+        </is>
+      </c>
+      <c r="G37" t="inlineStr">
+        <is>
+          <t>HOT WATER</t>
+        </is>
+      </c>
+      <c r="H37" t="inlineStr">
+        <is>
+          <t>Not Found</t>
+        </is>
+      </c>
+      <c r="I37" t="inlineStr">
+        <is>
+          <t>ASTM A36</t>
+        </is>
+      </c>
+      <c r="J37" t="inlineStr">
+        <is>
+          <t>A36</t>
+        </is>
+      </c>
+      <c r="K37" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="L37" t="inlineStr">
+        <is>
+          <t>120 °C</t>
+        </is>
+      </c>
+      <c r="M37" t="inlineStr">
+        <is>
+          <t>4 Bar</t>
+        </is>
+      </c>
+      <c r="N37" t="inlineStr">
+        <is>
+          <t>90 °C</t>
+        </is>
+      </c>
+      <c r="O37" t="inlineStr">
+        <is>
+          <t>1 Bar</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="E38" t="inlineStr">
+        <is>
+          <t>Angle Bar</t>
+        </is>
+      </c>
+      <c r="G38" t="inlineStr">
+        <is>
+          <t>HOT WATER</t>
+        </is>
+      </c>
+      <c r="H38" t="inlineStr">
+        <is>
+          <t>Not Found</t>
+        </is>
+      </c>
+      <c r="I38" t="inlineStr">
+        <is>
+          <t>ASTM A36</t>
+        </is>
+      </c>
+      <c r="J38" t="inlineStr">
+        <is>
+          <t>A36</t>
+        </is>
+      </c>
+      <c r="K38" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="L38" t="inlineStr">
+        <is>
+          <t>120 °C</t>
+        </is>
+      </c>
+      <c r="M38" t="inlineStr">
+        <is>
+          <t>4 Bar</t>
+        </is>
+      </c>
+      <c r="N38" t="inlineStr">
+        <is>
+          <t>90 °C</t>
+        </is>
+      </c>
+      <c r="O38" t="inlineStr">
+        <is>
+          <t>1 Bar</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="E39" t="inlineStr">
+        <is>
+          <t>Bracket 2</t>
+        </is>
+      </c>
+      <c r="G39" t="inlineStr">
+        <is>
+          <t>HOT WATER</t>
+        </is>
+      </c>
+      <c r="H39" t="inlineStr">
+        <is>
+          <t>Not Found</t>
+        </is>
+      </c>
+      <c r="I39" t="inlineStr">
+        <is>
+          <t>ASTM A36</t>
+        </is>
+      </c>
+      <c r="J39" t="inlineStr">
+        <is>
+          <t>A36</t>
+        </is>
+      </c>
+      <c r="K39" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="L39" t="inlineStr">
+        <is>
+          <t>120 °C</t>
+        </is>
+      </c>
+      <c r="M39" t="inlineStr">
+        <is>
+          <t>4 Bar</t>
+        </is>
+      </c>
+      <c r="N39" t="inlineStr">
+        <is>
+          <t>90 °C</t>
+        </is>
+      </c>
+      <c r="O39" t="inlineStr">
+        <is>
+          <t>1 Bar</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="E40" t="inlineStr">
+        <is>
+          <t>Bracket 3</t>
+        </is>
+      </c>
+      <c r="G40" t="inlineStr">
+        <is>
+          <t>HOT WATER</t>
+        </is>
+      </c>
+      <c r="H40" t="inlineStr">
+        <is>
+          <t>Not Found</t>
+        </is>
+      </c>
+      <c r="I40" t="inlineStr">
+        <is>
+          <t>ASTM A36</t>
+        </is>
+      </c>
+      <c r="J40" t="inlineStr">
+        <is>
+          <t>A36</t>
+        </is>
+      </c>
+      <c r="K40" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="L40" t="inlineStr">
+        <is>
+          <t>120 °C</t>
+        </is>
+      </c>
+      <c r="M40" t="inlineStr">
+        <is>
+          <t>4 Bar</t>
+        </is>
+      </c>
+      <c r="N40" t="inlineStr">
+        <is>
+          <t>90 °C</t>
+        </is>
+      </c>
+      <c r="O40" t="inlineStr">
+        <is>
+          <t>1 Bar</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="E41" t="inlineStr">
+        <is>
+          <t>Grating</t>
+        </is>
+      </c>
+      <c r="G41" t="inlineStr">
+        <is>
+          <t>HOT WATER</t>
+        </is>
+      </c>
+      <c r="H41" t="inlineStr">
+        <is>
+          <t>Not Found</t>
+        </is>
+      </c>
+      <c r="I41" t="inlineStr">
+        <is>
+          <t>ASTM A36</t>
+        </is>
+      </c>
+      <c r="J41" t="inlineStr">
+        <is>
+          <t>A36</t>
+        </is>
+      </c>
+      <c r="K41" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="L41" t="inlineStr">
+        <is>
+          <t>120 °C</t>
+        </is>
+      </c>
+      <c r="M41" t="inlineStr">
+        <is>
+          <t>4 Bar</t>
+        </is>
+      </c>
+      <c r="N41" t="inlineStr">
+        <is>
+          <t>90 °C</t>
+        </is>
+      </c>
+      <c r="O41" t="inlineStr">
+        <is>
+          <t>1 Bar</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="E42" t="inlineStr">
+        <is>
+          <t>Angle Bar</t>
+        </is>
+      </c>
+      <c r="G42" t="inlineStr">
+        <is>
+          <t>HOT WATER</t>
+        </is>
+      </c>
+      <c r="H42" t="inlineStr">
+        <is>
+          <t>Not Found</t>
+        </is>
+      </c>
+      <c r="I42" t="inlineStr">
+        <is>
+          <t>ASTM A36</t>
+        </is>
+      </c>
+      <c r="J42" t="inlineStr">
+        <is>
+          <t>A36</t>
+        </is>
+      </c>
+      <c r="K42" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="L42" t="inlineStr">
+        <is>
+          <t>120 °C</t>
+        </is>
+      </c>
+      <c r="M42" t="inlineStr">
+        <is>
+          <t>4 Bar</t>
+        </is>
+      </c>
+      <c r="N42" t="inlineStr">
+        <is>
+          <t>90 °C</t>
+        </is>
+      </c>
+      <c r="O42" t="inlineStr">
+        <is>
+          <t>1 Bar</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="E43" t="inlineStr">
+        <is>
+          <t>Angle Bar</t>
+        </is>
+      </c>
+      <c r="G43" t="inlineStr">
+        <is>
+          <t>HOT WATER</t>
+        </is>
+      </c>
+      <c r="H43" t="inlineStr">
+        <is>
+          <t>Not Found</t>
+        </is>
+      </c>
+      <c r="I43" t="inlineStr">
+        <is>
+          <t>ASTM A36</t>
+        </is>
+      </c>
+      <c r="J43" t="inlineStr">
+        <is>
+          <t>A36</t>
+        </is>
+      </c>
+      <c r="K43" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="L43" t="inlineStr">
+        <is>
+          <t>120 °C</t>
+        </is>
+      </c>
+      <c r="M43" t="inlineStr">
+        <is>
+          <t>4 Bar</t>
+        </is>
+      </c>
+      <c r="N43" t="inlineStr">
+        <is>
+          <t>90 °C</t>
+        </is>
+      </c>
+      <c r="O43" t="inlineStr">
+        <is>
+          <t>1 Bar</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="E44" t="inlineStr">
+        <is>
+          <t>Flat Plate</t>
+        </is>
+      </c>
+      <c r="G44" t="inlineStr">
+        <is>
+          <t>HOT WATER</t>
+        </is>
+      </c>
+      <c r="H44" t="inlineStr">
+        <is>
+          <t>Not Found</t>
+        </is>
+      </c>
+      <c r="I44" t="inlineStr">
+        <is>
+          <t>ASTM A36</t>
+        </is>
+      </c>
+      <c r="J44" t="inlineStr">
+        <is>
+          <t>A36</t>
+        </is>
+      </c>
+      <c r="K44" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="L44" t="inlineStr">
+        <is>
+          <t>120 °C</t>
+        </is>
+      </c>
+      <c r="M44" t="inlineStr">
+        <is>
+          <t>4 Bar</t>
+        </is>
+      </c>
+      <c r="N44" t="inlineStr">
+        <is>
+          <t>90 °C</t>
+        </is>
+      </c>
+      <c r="O44" t="inlineStr">
+        <is>
+          <t>1 Bar</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="E45" t="inlineStr">
+        <is>
+          <t>Flat Plate</t>
+        </is>
+      </c>
+      <c r="G45" t="inlineStr">
+        <is>
+          <t>HOT WATER</t>
+        </is>
+      </c>
+      <c r="H45" t="inlineStr">
+        <is>
+          <t>Not Found</t>
+        </is>
+      </c>
+      <c r="I45" t="inlineStr">
+        <is>
+          <t>ASTM A36</t>
+        </is>
+      </c>
+      <c r="J45" t="inlineStr">
+        <is>
+          <t>A36</t>
+        </is>
+      </c>
+      <c r="K45" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="L45" t="inlineStr">
+        <is>
+          <t>120 °C</t>
+        </is>
+      </c>
+      <c r="M45" t="inlineStr">
+        <is>
+          <t>4 Bar</t>
+        </is>
+      </c>
+      <c r="N45" t="inlineStr">
+        <is>
+          <t>90 °C</t>
+        </is>
+      </c>
+      <c r="O45" t="inlineStr">
+        <is>
+          <t>1 Bar</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="E46" t="inlineStr">
+        <is>
+          <t>Angle Bar</t>
+        </is>
+      </c>
+      <c r="G46" t="inlineStr">
+        <is>
+          <t>HOT WATER</t>
+        </is>
+      </c>
+      <c r="H46" t="inlineStr">
+        <is>
+          <t>Not Found</t>
+        </is>
+      </c>
+      <c r="I46" t="inlineStr">
+        <is>
+          <t>ASTM A36</t>
+        </is>
+      </c>
+      <c r="J46" t="inlineStr">
+        <is>
+          <t>A36</t>
+        </is>
+      </c>
+      <c r="K46" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="L46" t="inlineStr">
+        <is>
+          <t>120 °C</t>
+        </is>
+      </c>
+      <c r="M46" t="inlineStr">
+        <is>
+          <t>4 Bar</t>
+        </is>
+      </c>
+      <c r="N46" t="inlineStr">
+        <is>
+          <t>90 °C</t>
+        </is>
+      </c>
+      <c r="O46" t="inlineStr">
+        <is>
+          <t>1 Bar</t>
+        </is>
+      </c>
+    </row>
+    <row r="47">
+      <c r="E47" t="inlineStr">
+        <is>
+          <t>Angle Bar</t>
+        </is>
+      </c>
+      <c r="G47" t="inlineStr">
+        <is>
+          <t>HOT WATER</t>
+        </is>
+      </c>
+      <c r="H47" t="inlineStr">
+        <is>
+          <t>Not Found</t>
+        </is>
+      </c>
+      <c r="I47" t="inlineStr">
+        <is>
+          <t>ASTM A36</t>
+        </is>
+      </c>
+      <c r="J47" t="inlineStr">
+        <is>
+          <t>A36</t>
+        </is>
+      </c>
+      <c r="K47" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="L47" t="inlineStr">
+        <is>
+          <t>120 °C</t>
+        </is>
+      </c>
+      <c r="M47" t="inlineStr">
+        <is>
+          <t>4 Bar</t>
+        </is>
+      </c>
+      <c r="N47" t="inlineStr">
+        <is>
+          <t>90 °C</t>
+        </is>
+      </c>
+      <c r="O47" t="inlineStr">
+        <is>
+          <t>1 Bar</t>
+        </is>
+      </c>
+    </row>
+    <row r="48">
+      <c r="E48" t="inlineStr">
+        <is>
+          <t>Side Rail</t>
+        </is>
+      </c>
+      <c r="G48" t="inlineStr">
+        <is>
+          <t>HOT WATER</t>
+        </is>
+      </c>
+      <c r="H48" t="inlineStr">
+        <is>
+          <t>Not Found</t>
+        </is>
+      </c>
+      <c r="I48" t="inlineStr">
+        <is>
+          <t>ASTM A36</t>
+        </is>
+      </c>
+      <c r="J48" t="inlineStr">
+        <is>
+          <t>A36</t>
+        </is>
+      </c>
+      <c r="K48" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="L48" t="inlineStr">
+        <is>
+          <t>120 °C</t>
+        </is>
+      </c>
+      <c r="M48" t="inlineStr">
+        <is>
+          <t>4 Bar</t>
+        </is>
+      </c>
+      <c r="N48" t="inlineStr">
+        <is>
+          <t>90 °C</t>
+        </is>
+      </c>
+      <c r="O48" t="inlineStr">
+        <is>
+          <t>1 Bar</t>
+        </is>
+      </c>
+    </row>
+    <row r="49">
+      <c r="E49" t="inlineStr">
+        <is>
+          <t>Ladder Bracket</t>
+        </is>
+      </c>
+      <c r="G49" t="inlineStr">
+        <is>
+          <t>HOT WATER</t>
+        </is>
+      </c>
+      <c r="H49" t="inlineStr">
+        <is>
+          <t>Not Found</t>
+        </is>
+      </c>
+      <c r="I49" t="inlineStr">
+        <is>
+          <t>ASTM A36</t>
+        </is>
+      </c>
+      <c r="J49" t="inlineStr">
+        <is>
+          <t>A36</t>
+        </is>
+      </c>
+      <c r="K49" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="L49" t="inlineStr">
+        <is>
+          <t>120 °C</t>
+        </is>
+      </c>
+      <c r="M49" t="inlineStr">
+        <is>
+          <t>4 Bar</t>
+        </is>
+      </c>
+      <c r="N49" t="inlineStr">
+        <is>
+          <t>90 °C</t>
+        </is>
+      </c>
+      <c r="O49" t="inlineStr">
+        <is>
+          <t>1 Bar</t>
+        </is>
+      </c>
+    </row>
+    <row r="50">
+      <c r="E50" t="inlineStr">
+        <is>
+          <t>Round Bar</t>
+        </is>
+      </c>
+      <c r="G50" t="inlineStr">
+        <is>
+          <t>HOT WATER</t>
+        </is>
+      </c>
+      <c r="H50" t="inlineStr">
+        <is>
+          <t>Not Found</t>
+        </is>
+      </c>
+      <c r="I50" t="inlineStr">
+        <is>
+          <t>ASTM A36</t>
+        </is>
+      </c>
+      <c r="J50" t="inlineStr">
+        <is>
+          <t>A36</t>
+        </is>
+      </c>
+      <c r="K50" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="L50" t="inlineStr">
+        <is>
+          <t>120 °C</t>
+        </is>
+      </c>
+      <c r="M50" t="inlineStr">
+        <is>
+          <t>4 Bar</t>
+        </is>
+      </c>
+      <c r="N50" t="inlineStr">
+        <is>
+          <t>90 °C</t>
+        </is>
+      </c>
+      <c r="O50" t="inlineStr">
+        <is>
+          <t>1 Bar</t>
+        </is>
+      </c>
+    </row>
+    <row r="51">
+      <c r="E51" t="inlineStr">
+        <is>
+          <t>Saddle Support Plate</t>
+        </is>
+      </c>
+      <c r="G51" t="inlineStr">
+        <is>
+          <t>HOT WATER</t>
+        </is>
+      </c>
+      <c r="H51" t="inlineStr">
+        <is>
+          <t>Stainless Steel</t>
+        </is>
+      </c>
+      <c r="I51" t="inlineStr">
+        <is>
+          <t>ASTM A240</t>
+        </is>
+      </c>
+      <c r="J51" t="inlineStr">
+        <is>
+          <t>304L</t>
+        </is>
+      </c>
+      <c r="K51" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="L51" t="inlineStr">
+        <is>
+          <t>120 °C</t>
+        </is>
+      </c>
+      <c r="M51" t="inlineStr">
+        <is>
+          <t>4 Bar</t>
+        </is>
+      </c>
+      <c r="N51" t="inlineStr">
+        <is>
+          <t>90 °C</t>
+        </is>
+      </c>
+      <c r="O51" t="inlineStr">
+        <is>
+          <t>1 Bar</t>
+        </is>
+      </c>
+    </row>
+    <row r="52">
+      <c r="E52" t="inlineStr">
+        <is>
+          <t>Pad Plate</t>
+        </is>
+      </c>
+      <c r="G52" t="inlineStr">
+        <is>
+          <t>HOT WATER</t>
+        </is>
+      </c>
+      <c r="H52" t="inlineStr">
+        <is>
+          <t>Not Found</t>
+        </is>
+      </c>
+      <c r="I52" t="inlineStr">
+        <is>
+          <t>ASTM A36</t>
+        </is>
+      </c>
+      <c r="J52" t="inlineStr">
+        <is>
+          <t>A36</t>
+        </is>
+      </c>
+      <c r="K52" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="L52" t="inlineStr">
+        <is>
+          <t>120 °C</t>
+        </is>
+      </c>
+      <c r="M52" t="inlineStr">
+        <is>
+          <t>4 Bar</t>
+        </is>
+      </c>
+      <c r="N52" t="inlineStr">
+        <is>
+          <t>90 °C</t>
+        </is>
+      </c>
+      <c r="O52" t="inlineStr">
+        <is>
+          <t>1 Bar</t>
+        </is>
+      </c>
+    </row>
+    <row r="53">
+      <c r="E53" t="inlineStr">
+        <is>
+          <t>Pad Plate</t>
+        </is>
+      </c>
+      <c r="G53" t="inlineStr">
+        <is>
+          <t>HOT WATER</t>
+        </is>
+      </c>
+      <c r="H53" t="inlineStr">
+        <is>
+          <t>Not Found</t>
+        </is>
+      </c>
+      <c r="I53" t="inlineStr">
+        <is>
+          <t>ASTM A36</t>
+        </is>
+      </c>
+      <c r="J53" t="inlineStr">
+        <is>
+          <t>A36</t>
+        </is>
+      </c>
+      <c r="K53" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="L53" t="inlineStr">
+        <is>
+          <t>120 °C</t>
+        </is>
+      </c>
+      <c r="M53" t="inlineStr">
+        <is>
+          <t>4 Bar</t>
+        </is>
+      </c>
+      <c r="N53" t="inlineStr">
+        <is>
+          <t>90 °C</t>
+        </is>
+      </c>
+      <c r="O53" t="inlineStr">
+        <is>
+          <t>1 Bar</t>
         </is>
       </c>
     </row>
   </sheetData>
   <mergeCells count="19">
-    <mergeCell ref="A8:A21"/>
     <mergeCell ref="D5:D7"/>
-    <mergeCell ref="C8:C21"/>
     <mergeCell ref="B3:B4"/>
     <mergeCell ref="H5:J6"/>
     <mergeCell ref="A5:A7"/>
     <mergeCell ref="G5:G7"/>
-    <mergeCell ref="D8:D21"/>
     <mergeCell ref="B5:B7"/>
+    <mergeCell ref="B8:B53"/>
     <mergeCell ref="A3:A4"/>
     <mergeCell ref="D3:D4"/>
+    <mergeCell ref="A8:A53"/>
+    <mergeCell ref="C8:C53"/>
     <mergeCell ref="C5:C7"/>
     <mergeCell ref="E5:E7"/>
     <mergeCell ref="K5:K7"/>
     <mergeCell ref="F5:F7"/>
-    <mergeCell ref="B8:B21"/>
+    <mergeCell ref="D8:D53"/>
     <mergeCell ref="C3:C4"/>
     <mergeCell ref="L5:M6"/>
     <mergeCell ref="N5:O6"/>

</xml_diff>

<commit_message>
Added confidence level after each extraction
</commit_message>
<xml_diff>
--- a/outputs/10_output.xlsx
+++ b/outputs/10_output.xlsx
@@ -693,7 +693,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:O53"/>
+  <dimension ref="A1:O51"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A8" sqref="A8"/>
@@ -882,7 +882,11 @@
           <t>MLK_PMT_10104_-_V-004</t>
         </is>
       </c>
-      <c r="D8" s="29" t="inlineStr"/>
+      <c r="D8" s="29" t="inlineStr">
+        <is>
+          <t>Cooling of Water on Irrigation of An Absorber</t>
+        </is>
+      </c>
       <c r="E8" t="inlineStr">
         <is>
           <t>Shell Plate</t>
@@ -920,7 +924,7 @@
       </c>
       <c r="M8" t="inlineStr">
         <is>
-          <t>4 Bar</t>
+          <t>4 Bar G</t>
         </is>
       </c>
       <c r="N8" t="inlineStr">
@@ -930,7 +934,7 @@
       </c>
       <c r="O8" t="inlineStr">
         <is>
-          <t>1 Bar</t>
+          <t>1 Bar G</t>
         </is>
       </c>
     </row>
@@ -972,7 +976,7 @@
       </c>
       <c r="M9" t="inlineStr">
         <is>
-          <t>4 Bar</t>
+          <t>4 Bar G</t>
         </is>
       </c>
       <c r="N9" t="inlineStr">
@@ -982,7 +986,7 @@
       </c>
       <c r="O9" t="inlineStr">
         <is>
-          <t>1 Bar</t>
+          <t>1 Bar G</t>
         </is>
       </c>
     </row>
@@ -1024,7 +1028,7 @@
       </c>
       <c r="M10" t="inlineStr">
         <is>
-          <t>4 Bar</t>
+          <t>4 Bar G</t>
         </is>
       </c>
       <c r="N10" t="inlineStr">
@@ -1034,7 +1038,7 @@
       </c>
       <c r="O10" t="inlineStr">
         <is>
-          <t>1 Bar</t>
+          <t>1 Bar G</t>
         </is>
       </c>
     </row>
@@ -1076,7 +1080,7 @@
       </c>
       <c r="M11" t="inlineStr">
         <is>
-          <t>4 Bar</t>
+          <t>4 Bar G</t>
         </is>
       </c>
       <c r="N11" t="inlineStr">
@@ -1086,7 +1090,7 @@
       </c>
       <c r="O11" t="inlineStr">
         <is>
-          <t>1 Bar</t>
+          <t>1 Bar G</t>
         </is>
       </c>
     </row>
@@ -1128,7 +1132,7 @@
       </c>
       <c r="M12" t="inlineStr">
         <is>
-          <t>4 Bar</t>
+          <t>4 Bar G</t>
         </is>
       </c>
       <c r="N12" t="inlineStr">
@@ -1138,7 +1142,7 @@
       </c>
       <c r="O12" t="inlineStr">
         <is>
-          <t>1 Bar</t>
+          <t>1 Bar G</t>
         </is>
       </c>
     </row>
@@ -1180,7 +1184,7 @@
       </c>
       <c r="M13" t="inlineStr">
         <is>
-          <t>4 Bar</t>
+          <t>4 Bar G</t>
         </is>
       </c>
       <c r="N13" t="inlineStr">
@@ -1190,7 +1194,7 @@
       </c>
       <c r="O13" t="inlineStr">
         <is>
-          <t>1 Bar</t>
+          <t>1 Bar G</t>
         </is>
       </c>
     </row>
@@ -1232,7 +1236,7 @@
       </c>
       <c r="M14" t="inlineStr">
         <is>
-          <t>4 Bar</t>
+          <t>4 Bar G</t>
         </is>
       </c>
       <c r="N14" t="inlineStr">
@@ -1242,7 +1246,7 @@
       </c>
       <c r="O14" t="inlineStr">
         <is>
-          <t>1 Bar</t>
+          <t>1 Bar G</t>
         </is>
       </c>
     </row>
@@ -1284,7 +1288,7 @@
       </c>
       <c r="M15" t="inlineStr">
         <is>
-          <t>4 Bar</t>
+          <t>4 Bar G</t>
         </is>
       </c>
       <c r="N15" t="inlineStr">
@@ -1294,7 +1298,7 @@
       </c>
       <c r="O15" t="inlineStr">
         <is>
-          <t>1 Bar</t>
+          <t>1 Bar G</t>
         </is>
       </c>
     </row>
@@ -1336,7 +1340,7 @@
       </c>
       <c r="M16" t="inlineStr">
         <is>
-          <t>4 Bar</t>
+          <t>4 Bar G</t>
         </is>
       </c>
       <c r="N16" t="inlineStr">
@@ -1346,7 +1350,7 @@
       </c>
       <c r="O16" t="inlineStr">
         <is>
-          <t>1 Bar</t>
+          <t>1 Bar G</t>
         </is>
       </c>
     </row>
@@ -1388,7 +1392,7 @@
       </c>
       <c r="M17" t="inlineStr">
         <is>
-          <t>4 Bar</t>
+          <t>4 Bar G</t>
         </is>
       </c>
       <c r="N17" t="inlineStr">
@@ -1398,7 +1402,7 @@
       </c>
       <c r="O17" t="inlineStr">
         <is>
-          <t>1 Bar</t>
+          <t>1 Bar G</t>
         </is>
       </c>
     </row>
@@ -1440,7 +1444,7 @@
       </c>
       <c r="M18" t="inlineStr">
         <is>
-          <t>4 Bar</t>
+          <t>4 Bar G</t>
         </is>
       </c>
       <c r="N18" t="inlineStr">
@@ -1450,7 +1454,7 @@
       </c>
       <c r="O18" t="inlineStr">
         <is>
-          <t>1 Bar</t>
+          <t>1 Bar G</t>
         </is>
       </c>
     </row>
@@ -1492,7 +1496,7 @@
       </c>
       <c r="M19" t="inlineStr">
         <is>
-          <t>4 Bar</t>
+          <t>4 Bar G</t>
         </is>
       </c>
       <c r="N19" t="inlineStr">
@@ -1502,7 +1506,7 @@
       </c>
       <c r="O19" t="inlineStr">
         <is>
-          <t>1 Bar</t>
+          <t>1 Bar G</t>
         </is>
       </c>
     </row>
@@ -1544,7 +1548,7 @@
       </c>
       <c r="M20" t="inlineStr">
         <is>
-          <t>4 Bar</t>
+          <t>4 Bar G</t>
         </is>
       </c>
       <c r="N20" t="inlineStr">
@@ -1554,7 +1558,7 @@
       </c>
       <c r="O20" t="inlineStr">
         <is>
-          <t>1 Bar</t>
+          <t>1 Bar G</t>
         </is>
       </c>
     </row>
@@ -1596,7 +1600,7 @@
       </c>
       <c r="M21" t="inlineStr">
         <is>
-          <t>4 Bar</t>
+          <t>4 Bar G</t>
         </is>
       </c>
       <c r="N21" t="inlineStr">
@@ -1606,7 +1610,7 @@
       </c>
       <c r="O21" t="inlineStr">
         <is>
-          <t>1 Bar</t>
+          <t>1 Bar G</t>
         </is>
       </c>
     </row>
@@ -1648,7 +1652,7 @@
       </c>
       <c r="M22" t="inlineStr">
         <is>
-          <t>4 Bar</t>
+          <t>4 Bar G</t>
         </is>
       </c>
       <c r="N22" t="inlineStr">
@@ -1658,7 +1662,7 @@
       </c>
       <c r="O22" t="inlineStr">
         <is>
-          <t>1 Bar</t>
+          <t>1 Bar G</t>
         </is>
       </c>
     </row>
@@ -1700,7 +1704,7 @@
       </c>
       <c r="M23" t="inlineStr">
         <is>
-          <t>4 Bar</t>
+          <t>4 Bar G</t>
         </is>
       </c>
       <c r="N23" t="inlineStr">
@@ -1710,14 +1714,14 @@
       </c>
       <c r="O23" t="inlineStr">
         <is>
-          <t>1 Bar</t>
+          <t>1 Bar G</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="E24" t="inlineStr">
         <is>
-          <t>Flange</t>
+          <t>Neck</t>
         </is>
       </c>
       <c r="G24" t="inlineStr">
@@ -1732,12 +1736,12 @@
       </c>
       <c r="I24" t="inlineStr">
         <is>
-          <t>ASTM A182</t>
+          <t>ASTM A312</t>
         </is>
       </c>
       <c r="J24" t="inlineStr">
         <is>
-          <t>F304L</t>
+          <t>TP304L</t>
         </is>
       </c>
       <c r="K24" t="inlineStr">
@@ -1752,7 +1756,7 @@
       </c>
       <c r="M24" t="inlineStr">
         <is>
-          <t>4 Bar</t>
+          <t>4 Bar G</t>
         </is>
       </c>
       <c r="N24" t="inlineStr">
@@ -1762,7 +1766,7 @@
       </c>
       <c r="O24" t="inlineStr">
         <is>
-          <t>1 Bar</t>
+          <t>1 Bar G</t>
         </is>
       </c>
     </row>
@@ -1804,7 +1808,7 @@
       </c>
       <c r="M25" t="inlineStr">
         <is>
-          <t>4 Bar</t>
+          <t>4 Bar G</t>
         </is>
       </c>
       <c r="N25" t="inlineStr">
@@ -1814,14 +1818,14 @@
       </c>
       <c r="O25" t="inlineStr">
         <is>
-          <t>1 Bar</t>
+          <t>1 Bar G</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="E26" t="inlineStr">
         <is>
-          <t>Neck</t>
+          <t>Flange</t>
         </is>
       </c>
       <c r="G26" t="inlineStr">
@@ -1836,12 +1840,12 @@
       </c>
       <c r="I26" t="inlineStr">
         <is>
-          <t>ASTM A312</t>
+          <t>ASTM A182</t>
         </is>
       </c>
       <c r="J26" t="inlineStr">
         <is>
-          <t>TP304L</t>
+          <t>F304L</t>
         </is>
       </c>
       <c r="K26" t="inlineStr">
@@ -1856,7 +1860,7 @@
       </c>
       <c r="M26" t="inlineStr">
         <is>
-          <t>4 Bar</t>
+          <t>4 Bar G</t>
         </is>
       </c>
       <c r="N26" t="inlineStr">
@@ -1866,14 +1870,14 @@
       </c>
       <c r="O26" t="inlineStr">
         <is>
-          <t>1 Bar</t>
+          <t>1 Bar G</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="E27" t="inlineStr">
         <is>
-          <t>Flange</t>
+          <t>Neck</t>
         </is>
       </c>
       <c r="G27" t="inlineStr">
@@ -1888,12 +1892,12 @@
       </c>
       <c r="I27" t="inlineStr">
         <is>
-          <t>ASTM A182</t>
+          <t>ASTM A312</t>
         </is>
       </c>
       <c r="J27" t="inlineStr">
         <is>
-          <t>F304L</t>
+          <t>TP304L</t>
         </is>
       </c>
       <c r="K27" t="inlineStr">
@@ -1908,7 +1912,7 @@
       </c>
       <c r="M27" t="inlineStr">
         <is>
-          <t>4 Bar</t>
+          <t>4 Bar G</t>
         </is>
       </c>
       <c r="N27" t="inlineStr">
@@ -1918,14 +1922,14 @@
       </c>
       <c r="O27" t="inlineStr">
         <is>
-          <t>1 Bar</t>
+          <t>1 Bar G</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="E28" t="inlineStr">
         <is>
-          <t>Flange</t>
+          <t>Neck</t>
         </is>
       </c>
       <c r="G28" t="inlineStr">
@@ -1940,12 +1944,12 @@
       </c>
       <c r="I28" t="inlineStr">
         <is>
-          <t>ASTM A182</t>
+          <t>ASTM A312</t>
         </is>
       </c>
       <c r="J28" t="inlineStr">
         <is>
-          <t>F304L</t>
+          <t>TP304L</t>
         </is>
       </c>
       <c r="K28" t="inlineStr">
@@ -1960,7 +1964,7 @@
       </c>
       <c r="M28" t="inlineStr">
         <is>
-          <t>4 Bar</t>
+          <t>4 Bar G</t>
         </is>
       </c>
       <c r="N28" t="inlineStr">
@@ -1970,14 +1974,14 @@
       </c>
       <c r="O28" t="inlineStr">
         <is>
-          <t>1 Bar</t>
+          <t>1 Bar G</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="E29" t="inlineStr">
         <is>
-          <t>Neck</t>
+          <t>Blind Flange</t>
         </is>
       </c>
       <c r="G29" t="inlineStr">
@@ -1992,12 +1996,12 @@
       </c>
       <c r="I29" t="inlineStr">
         <is>
-          <t>ASTM A312</t>
+          <t>ASTM A182</t>
         </is>
       </c>
       <c r="J29" t="inlineStr">
         <is>
-          <t>TP304L</t>
+          <t>F304L</t>
         </is>
       </c>
       <c r="K29" t="inlineStr">
@@ -2012,7 +2016,7 @@
       </c>
       <c r="M29" t="inlineStr">
         <is>
-          <t>4 Bar</t>
+          <t>4 Bar G</t>
         </is>
       </c>
       <c r="N29" t="inlineStr">
@@ -2022,14 +2026,14 @@
       </c>
       <c r="O29" t="inlineStr">
         <is>
-          <t>1 Bar</t>
+          <t>1 Bar G</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="E30" t="inlineStr">
         <is>
-          <t>Neck</t>
+          <t>Spiral Wound Gasket</t>
         </is>
       </c>
       <c r="G30" t="inlineStr">
@@ -2044,12 +2048,12 @@
       </c>
       <c r="I30" t="inlineStr">
         <is>
-          <t>ASTM A312</t>
+          <t>ASTM A182</t>
         </is>
       </c>
       <c r="J30" t="inlineStr">
         <is>
-          <t>TP304L</t>
+          <t>F304L</t>
         </is>
       </c>
       <c r="K30" t="inlineStr">
@@ -2064,7 +2068,7 @@
       </c>
       <c r="M30" t="inlineStr">
         <is>
-          <t>4 Bar</t>
+          <t>4 Bar G</t>
         </is>
       </c>
       <c r="N30" t="inlineStr">
@@ -2074,14 +2078,14 @@
       </c>
       <c r="O30" t="inlineStr">
         <is>
-          <t>1 Bar</t>
+          <t>1 Bar G</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="E31" t="inlineStr">
         <is>
-          <t>Blind Flange</t>
+          <t>Flange</t>
         </is>
       </c>
       <c r="G31" t="inlineStr">
@@ -2116,7 +2120,7 @@
       </c>
       <c r="M31" t="inlineStr">
         <is>
-          <t>4 Bar</t>
+          <t>4 Bar G</t>
         </is>
       </c>
       <c r="N31" t="inlineStr">
@@ -2126,14 +2130,14 @@
       </c>
       <c r="O31" t="inlineStr">
         <is>
-          <t>1 Bar</t>
+          <t>1 Bar G</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="E32" t="inlineStr">
         <is>
-          <t>Spiral Wound Gasket</t>
+          <t>Neck</t>
         </is>
       </c>
       <c r="G32" t="inlineStr">
@@ -2143,12 +2147,17 @@
       </c>
       <c r="H32" t="inlineStr">
         <is>
-          <t>Not Found</t>
+          <t>Stainless Steel</t>
         </is>
       </c>
       <c r="I32" t="inlineStr">
         <is>
-          <t>ASME B16.20</t>
+          <t>ASTM A240</t>
+        </is>
+      </c>
+      <c r="J32" t="inlineStr">
+        <is>
+          <t>304L</t>
         </is>
       </c>
       <c r="K32" t="inlineStr">
@@ -2163,7 +2172,7 @@
       </c>
       <c r="M32" t="inlineStr">
         <is>
-          <t>4 Bar</t>
+          <t>4 Bar G</t>
         </is>
       </c>
       <c r="N32" t="inlineStr">
@@ -2173,14 +2182,14 @@
       </c>
       <c r="O32" t="inlineStr">
         <is>
-          <t>1 Bar</t>
+          <t>1 Bar G</t>
         </is>
       </c>
     </row>
     <row r="33">
       <c r="E33" t="inlineStr">
         <is>
-          <t>Flange</t>
+          <t>Stud Bolt</t>
         </is>
       </c>
       <c r="G33" t="inlineStr">
@@ -2190,17 +2199,17 @@
       </c>
       <c r="H33" t="inlineStr">
         <is>
-          <t>Stainless Steel</t>
+          <t>Stainless Steel Bolting</t>
         </is>
       </c>
       <c r="I33" t="inlineStr">
         <is>
-          <t>ASTM A182</t>
+          <t>ASTM A193</t>
         </is>
       </c>
       <c r="J33" t="inlineStr">
         <is>
-          <t>F304L</t>
+          <t>GR B8M</t>
         </is>
       </c>
       <c r="K33" t="inlineStr">
@@ -2215,7 +2224,7 @@
       </c>
       <c r="M33" t="inlineStr">
         <is>
-          <t>4 Bar</t>
+          <t>4 Bar G</t>
         </is>
       </c>
       <c r="N33" t="inlineStr">
@@ -2225,14 +2234,14 @@
       </c>
       <c r="O33" t="inlineStr">
         <is>
-          <t>1 Bar</t>
+          <t>1 Bar G</t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="E34" t="inlineStr">
         <is>
-          <t>Neck</t>
+          <t>Nuts &amp; Washer</t>
         </is>
       </c>
       <c r="G34" t="inlineStr">
@@ -2242,17 +2251,17 @@
       </c>
       <c r="H34" t="inlineStr">
         <is>
-          <t>Stainless Steel</t>
+          <t>Heavy Hex Nuts</t>
         </is>
       </c>
       <c r="I34" t="inlineStr">
         <is>
-          <t>ASTM A312</t>
+          <t>ASTM A194</t>
         </is>
       </c>
       <c r="J34" t="inlineStr">
         <is>
-          <t>TP304L</t>
+          <t>GR 2H</t>
         </is>
       </c>
       <c r="K34" t="inlineStr">
@@ -2267,7 +2276,7 @@
       </c>
       <c r="M34" t="inlineStr">
         <is>
-          <t>4 Bar</t>
+          <t>4 Bar G</t>
         </is>
       </c>
       <c r="N34" t="inlineStr">
@@ -2277,14 +2286,14 @@
       </c>
       <c r="O34" t="inlineStr">
         <is>
-          <t>1 Bar</t>
+          <t>1 Bar G</t>
         </is>
       </c>
     </row>
     <row r="35">
       <c r="E35" t="inlineStr">
         <is>
-          <t>Stud Bolt</t>
+          <t>Bracket 1</t>
         </is>
       </c>
       <c r="G35" t="inlineStr">
@@ -2294,17 +2303,12 @@
       </c>
       <c r="H35" t="inlineStr">
         <is>
-          <t>Stainless Steel Bolting</t>
+          <t>Not Found</t>
         </is>
       </c>
       <c r="I35" t="inlineStr">
         <is>
-          <t>ASTM A193</t>
-        </is>
-      </c>
-      <c r="J35" t="inlineStr">
-        <is>
-          <t>B8M</t>
+          <t>ASTM A36</t>
         </is>
       </c>
       <c r="K35" t="inlineStr">
@@ -2319,7 +2323,7 @@
       </c>
       <c r="M35" t="inlineStr">
         <is>
-          <t>4 Bar</t>
+          <t>4 Bar G</t>
         </is>
       </c>
       <c r="N35" t="inlineStr">
@@ -2329,14 +2333,14 @@
       </c>
       <c r="O35" t="inlineStr">
         <is>
-          <t>1 Bar</t>
+          <t>1 Bar G</t>
         </is>
       </c>
     </row>
     <row r="36">
       <c r="E36" t="inlineStr">
         <is>
-          <t>Nuts &amp; Washer</t>
+          <t>Angle Bar</t>
         </is>
       </c>
       <c r="G36" t="inlineStr">
@@ -2346,17 +2350,12 @@
       </c>
       <c r="H36" t="inlineStr">
         <is>
-          <t>Heavy Hex Nuts</t>
+          <t>Not Found</t>
         </is>
       </c>
       <c r="I36" t="inlineStr">
         <is>
-          <t>ASTM A194</t>
-        </is>
-      </c>
-      <c r="J36" t="inlineStr">
-        <is>
-          <t>2H</t>
+          <t>ASTM A36</t>
         </is>
       </c>
       <c r="K36" t="inlineStr">
@@ -2371,7 +2370,7 @@
       </c>
       <c r="M36" t="inlineStr">
         <is>
-          <t>4 Bar</t>
+          <t>4 Bar G</t>
         </is>
       </c>
       <c r="N36" t="inlineStr">
@@ -2381,14 +2380,14 @@
       </c>
       <c r="O36" t="inlineStr">
         <is>
-          <t>1 Bar</t>
+          <t>1 Bar G</t>
         </is>
       </c>
     </row>
     <row r="37">
       <c r="E37" t="inlineStr">
         <is>
-          <t>Bracket 1</t>
+          <t>Bracket 2</t>
         </is>
       </c>
       <c r="G37" t="inlineStr">
@@ -2406,11 +2405,6 @@
           <t>ASTM A36</t>
         </is>
       </c>
-      <c r="J37" t="inlineStr">
-        <is>
-          <t>A36</t>
-        </is>
-      </c>
       <c r="K37" t="inlineStr">
         <is>
           <t>N/A</t>
@@ -2423,7 +2417,7 @@
       </c>
       <c r="M37" t="inlineStr">
         <is>
-          <t>4 Bar</t>
+          <t>4 Bar G</t>
         </is>
       </c>
       <c r="N37" t="inlineStr">
@@ -2433,14 +2427,14 @@
       </c>
       <c r="O37" t="inlineStr">
         <is>
-          <t>1 Bar</t>
+          <t>1 Bar G</t>
         </is>
       </c>
     </row>
     <row r="38">
       <c r="E38" t="inlineStr">
         <is>
-          <t>Angle Bar</t>
+          <t>Bracket 3</t>
         </is>
       </c>
       <c r="G38" t="inlineStr">
@@ -2458,11 +2452,6 @@
           <t>ASTM A36</t>
         </is>
       </c>
-      <c r="J38" t="inlineStr">
-        <is>
-          <t>A36</t>
-        </is>
-      </c>
       <c r="K38" t="inlineStr">
         <is>
           <t>N/A</t>
@@ -2475,7 +2464,7 @@
       </c>
       <c r="M38" t="inlineStr">
         <is>
-          <t>4 Bar</t>
+          <t>4 Bar G</t>
         </is>
       </c>
       <c r="N38" t="inlineStr">
@@ -2485,14 +2474,14 @@
       </c>
       <c r="O38" t="inlineStr">
         <is>
-          <t>1 Bar</t>
+          <t>1 Bar G</t>
         </is>
       </c>
     </row>
     <row r="39">
       <c r="E39" t="inlineStr">
         <is>
-          <t>Bracket 2</t>
+          <t>Grating</t>
         </is>
       </c>
       <c r="G39" t="inlineStr">
@@ -2510,11 +2499,6 @@
           <t>ASTM A36</t>
         </is>
       </c>
-      <c r="J39" t="inlineStr">
-        <is>
-          <t>A36</t>
-        </is>
-      </c>
       <c r="K39" t="inlineStr">
         <is>
           <t>N/A</t>
@@ -2527,7 +2511,7 @@
       </c>
       <c r="M39" t="inlineStr">
         <is>
-          <t>4 Bar</t>
+          <t>4 Bar G</t>
         </is>
       </c>
       <c r="N39" t="inlineStr">
@@ -2537,14 +2521,14 @@
       </c>
       <c r="O39" t="inlineStr">
         <is>
-          <t>1 Bar</t>
+          <t>1 Bar G</t>
         </is>
       </c>
     </row>
     <row r="40">
       <c r="E40" t="inlineStr">
         <is>
-          <t>Bracket 3</t>
+          <t>Angle Bar</t>
         </is>
       </c>
       <c r="G40" t="inlineStr">
@@ -2562,11 +2546,6 @@
           <t>ASTM A36</t>
         </is>
       </c>
-      <c r="J40" t="inlineStr">
-        <is>
-          <t>A36</t>
-        </is>
-      </c>
       <c r="K40" t="inlineStr">
         <is>
           <t>N/A</t>
@@ -2579,7 +2558,7 @@
       </c>
       <c r="M40" t="inlineStr">
         <is>
-          <t>4 Bar</t>
+          <t>4 Bar G</t>
         </is>
       </c>
       <c r="N40" t="inlineStr">
@@ -2589,14 +2568,14 @@
       </c>
       <c r="O40" t="inlineStr">
         <is>
-          <t>1 Bar</t>
+          <t>1 Bar G</t>
         </is>
       </c>
     </row>
     <row r="41">
       <c r="E41" t="inlineStr">
         <is>
-          <t>Grating</t>
+          <t>Angle Bar</t>
         </is>
       </c>
       <c r="G41" t="inlineStr">
@@ -2614,11 +2593,6 @@
           <t>ASTM A36</t>
         </is>
       </c>
-      <c r="J41" t="inlineStr">
-        <is>
-          <t>A36</t>
-        </is>
-      </c>
       <c r="K41" t="inlineStr">
         <is>
           <t>N/A</t>
@@ -2631,7 +2605,7 @@
       </c>
       <c r="M41" t="inlineStr">
         <is>
-          <t>4 Bar</t>
+          <t>4 Bar G</t>
         </is>
       </c>
       <c r="N41" t="inlineStr">
@@ -2641,14 +2615,14 @@
       </c>
       <c r="O41" t="inlineStr">
         <is>
-          <t>1 Bar</t>
+          <t>1 Bar G</t>
         </is>
       </c>
     </row>
     <row r="42">
       <c r="E42" t="inlineStr">
         <is>
-          <t>Angle Bar</t>
+          <t>Flat Plate</t>
         </is>
       </c>
       <c r="G42" t="inlineStr">
@@ -2666,11 +2640,6 @@
           <t>ASTM A36</t>
         </is>
       </c>
-      <c r="J42" t="inlineStr">
-        <is>
-          <t>A36</t>
-        </is>
-      </c>
       <c r="K42" t="inlineStr">
         <is>
           <t>N/A</t>
@@ -2683,7 +2652,7 @@
       </c>
       <c r="M42" t="inlineStr">
         <is>
-          <t>4 Bar</t>
+          <t>4 Bar G</t>
         </is>
       </c>
       <c r="N42" t="inlineStr">
@@ -2693,14 +2662,14 @@
       </c>
       <c r="O42" t="inlineStr">
         <is>
-          <t>1 Bar</t>
+          <t>1 Bar G</t>
         </is>
       </c>
     </row>
     <row r="43">
       <c r="E43" t="inlineStr">
         <is>
-          <t>Angle Bar</t>
+          <t>Flat Plate</t>
         </is>
       </c>
       <c r="G43" t="inlineStr">
@@ -2718,11 +2687,6 @@
           <t>ASTM A36</t>
         </is>
       </c>
-      <c r="J43" t="inlineStr">
-        <is>
-          <t>A36</t>
-        </is>
-      </c>
       <c r="K43" t="inlineStr">
         <is>
           <t>N/A</t>
@@ -2735,7 +2699,7 @@
       </c>
       <c r="M43" t="inlineStr">
         <is>
-          <t>4 Bar</t>
+          <t>4 Bar G</t>
         </is>
       </c>
       <c r="N43" t="inlineStr">
@@ -2745,14 +2709,14 @@
       </c>
       <c r="O43" t="inlineStr">
         <is>
-          <t>1 Bar</t>
+          <t>1 Bar G</t>
         </is>
       </c>
     </row>
     <row r="44">
       <c r="E44" t="inlineStr">
         <is>
-          <t>Flat Plate</t>
+          <t>Angle Bar</t>
         </is>
       </c>
       <c r="G44" t="inlineStr">
@@ -2770,11 +2734,6 @@
           <t>ASTM A36</t>
         </is>
       </c>
-      <c r="J44" t="inlineStr">
-        <is>
-          <t>A36</t>
-        </is>
-      </c>
       <c r="K44" t="inlineStr">
         <is>
           <t>N/A</t>
@@ -2787,7 +2746,7 @@
       </c>
       <c r="M44" t="inlineStr">
         <is>
-          <t>4 Bar</t>
+          <t>4 Bar G</t>
         </is>
       </c>
       <c r="N44" t="inlineStr">
@@ -2797,14 +2756,14 @@
       </c>
       <c r="O44" t="inlineStr">
         <is>
-          <t>1 Bar</t>
+          <t>1 Bar G</t>
         </is>
       </c>
     </row>
     <row r="45">
       <c r="E45" t="inlineStr">
         <is>
-          <t>Flat Plate</t>
+          <t>Angle Bar</t>
         </is>
       </c>
       <c r="G45" t="inlineStr">
@@ -2822,11 +2781,6 @@
           <t>ASTM A36</t>
         </is>
       </c>
-      <c r="J45" t="inlineStr">
-        <is>
-          <t>A36</t>
-        </is>
-      </c>
       <c r="K45" t="inlineStr">
         <is>
           <t>N/A</t>
@@ -2839,7 +2793,7 @@
       </c>
       <c r="M45" t="inlineStr">
         <is>
-          <t>4 Bar</t>
+          <t>4 Bar G</t>
         </is>
       </c>
       <c r="N45" t="inlineStr">
@@ -2849,14 +2803,14 @@
       </c>
       <c r="O45" t="inlineStr">
         <is>
-          <t>1 Bar</t>
+          <t>1 Bar G</t>
         </is>
       </c>
     </row>
     <row r="46">
       <c r="E46" t="inlineStr">
         <is>
-          <t>Angle Bar</t>
+          <t>Side Rail</t>
         </is>
       </c>
       <c r="G46" t="inlineStr">
@@ -2874,11 +2828,6 @@
           <t>ASTM A36</t>
         </is>
       </c>
-      <c r="J46" t="inlineStr">
-        <is>
-          <t>A36</t>
-        </is>
-      </c>
       <c r="K46" t="inlineStr">
         <is>
           <t>N/A</t>
@@ -2891,7 +2840,7 @@
       </c>
       <c r="M46" t="inlineStr">
         <is>
-          <t>4 Bar</t>
+          <t>4 Bar G</t>
         </is>
       </c>
       <c r="N46" t="inlineStr">
@@ -2901,14 +2850,14 @@
       </c>
       <c r="O46" t="inlineStr">
         <is>
-          <t>1 Bar</t>
+          <t>1 Bar G</t>
         </is>
       </c>
     </row>
     <row r="47">
       <c r="E47" t="inlineStr">
         <is>
-          <t>Angle Bar</t>
+          <t>Ladder Bracket</t>
         </is>
       </c>
       <c r="G47" t="inlineStr">
@@ -2926,11 +2875,6 @@
           <t>ASTM A36</t>
         </is>
       </c>
-      <c r="J47" t="inlineStr">
-        <is>
-          <t>A36</t>
-        </is>
-      </c>
       <c r="K47" t="inlineStr">
         <is>
           <t>N/A</t>
@@ -2943,7 +2887,7 @@
       </c>
       <c r="M47" t="inlineStr">
         <is>
-          <t>4 Bar</t>
+          <t>4 Bar G</t>
         </is>
       </c>
       <c r="N47" t="inlineStr">
@@ -2953,14 +2897,14 @@
       </c>
       <c r="O47" t="inlineStr">
         <is>
-          <t>1 Bar</t>
+          <t>1 Bar G</t>
         </is>
       </c>
     </row>
     <row r="48">
       <c r="E48" t="inlineStr">
         <is>
-          <t>Side Rail</t>
+          <t>Round Bar</t>
         </is>
       </c>
       <c r="G48" t="inlineStr">
@@ -2978,11 +2922,6 @@
           <t>ASTM A36</t>
         </is>
       </c>
-      <c r="J48" t="inlineStr">
-        <is>
-          <t>A36</t>
-        </is>
-      </c>
       <c r="K48" t="inlineStr">
         <is>
           <t>N/A</t>
@@ -2995,7 +2934,7 @@
       </c>
       <c r="M48" t="inlineStr">
         <is>
-          <t>4 Bar</t>
+          <t>4 Bar G</t>
         </is>
       </c>
       <c r="N48" t="inlineStr">
@@ -3005,14 +2944,14 @@
       </c>
       <c r="O48" t="inlineStr">
         <is>
-          <t>1 Bar</t>
+          <t>1 Bar G</t>
         </is>
       </c>
     </row>
     <row r="49">
       <c r="E49" t="inlineStr">
         <is>
-          <t>Ladder Bracket</t>
+          <t>Saddle Support Plate</t>
         </is>
       </c>
       <c r="G49" t="inlineStr">
@@ -3022,17 +2961,17 @@
       </c>
       <c r="H49" t="inlineStr">
         <is>
-          <t>Not Found</t>
+          <t>Stainless Steel</t>
         </is>
       </c>
       <c r="I49" t="inlineStr">
         <is>
-          <t>ASTM A36</t>
+          <t>ASTM A240</t>
         </is>
       </c>
       <c r="J49" t="inlineStr">
         <is>
-          <t>A36</t>
+          <t>304L</t>
         </is>
       </c>
       <c r="K49" t="inlineStr">
@@ -3047,7 +2986,7 @@
       </c>
       <c r="M49" t="inlineStr">
         <is>
-          <t>4 Bar</t>
+          <t>4 Bar G</t>
         </is>
       </c>
       <c r="N49" t="inlineStr">
@@ -3057,14 +2996,14 @@
       </c>
       <c r="O49" t="inlineStr">
         <is>
-          <t>1 Bar</t>
+          <t>1 Bar G</t>
         </is>
       </c>
     </row>
     <row r="50">
       <c r="E50" t="inlineStr">
         <is>
-          <t>Round Bar</t>
+          <t>Pad Plate</t>
         </is>
       </c>
       <c r="G50" t="inlineStr">
@@ -3082,11 +3021,6 @@
           <t>ASTM A36</t>
         </is>
       </c>
-      <c r="J50" t="inlineStr">
-        <is>
-          <t>A36</t>
-        </is>
-      </c>
       <c r="K50" t="inlineStr">
         <is>
           <t>N/A</t>
@@ -3099,7 +3033,7 @@
       </c>
       <c r="M50" t="inlineStr">
         <is>
-          <t>4 Bar</t>
+          <t>4 Bar G</t>
         </is>
       </c>
       <c r="N50" t="inlineStr">
@@ -3109,14 +3043,14 @@
       </c>
       <c r="O50" t="inlineStr">
         <is>
-          <t>1 Bar</t>
+          <t>1 Bar G</t>
         </is>
       </c>
     </row>
     <row r="51">
       <c r="E51" t="inlineStr">
         <is>
-          <t>Saddle Support Plate</t>
+          <t>Pad Plate</t>
         </is>
       </c>
       <c r="G51" t="inlineStr">
@@ -3126,17 +3060,12 @@
       </c>
       <c r="H51" t="inlineStr">
         <is>
-          <t>Stainless Steel</t>
+          <t>Not Found</t>
         </is>
       </c>
       <c r="I51" t="inlineStr">
         <is>
-          <t>ASTM A240</t>
-        </is>
-      </c>
-      <c r="J51" t="inlineStr">
-        <is>
-          <t>304L</t>
+          <t>ASTM A36</t>
         </is>
       </c>
       <c r="K51" t="inlineStr">
@@ -3151,7 +3080,7 @@
       </c>
       <c r="M51" t="inlineStr">
         <is>
-          <t>4 Bar</t>
+          <t>4 Bar G</t>
         </is>
       </c>
       <c r="N51" t="inlineStr">
@@ -3161,111 +3090,7 @@
       </c>
       <c r="O51" t="inlineStr">
         <is>
-          <t>1 Bar</t>
-        </is>
-      </c>
-    </row>
-    <row r="52">
-      <c r="E52" t="inlineStr">
-        <is>
-          <t>Pad Plate</t>
-        </is>
-      </c>
-      <c r="G52" t="inlineStr">
-        <is>
-          <t>HOT WATER</t>
-        </is>
-      </c>
-      <c r="H52" t="inlineStr">
-        <is>
-          <t>Not Found</t>
-        </is>
-      </c>
-      <c r="I52" t="inlineStr">
-        <is>
-          <t>ASTM A36</t>
-        </is>
-      </c>
-      <c r="J52" t="inlineStr">
-        <is>
-          <t>A36</t>
-        </is>
-      </c>
-      <c r="K52" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-      <c r="L52" t="inlineStr">
-        <is>
-          <t>120 °C</t>
-        </is>
-      </c>
-      <c r="M52" t="inlineStr">
-        <is>
-          <t>4 Bar</t>
-        </is>
-      </c>
-      <c r="N52" t="inlineStr">
-        <is>
-          <t>90 °C</t>
-        </is>
-      </c>
-      <c r="O52" t="inlineStr">
-        <is>
-          <t>1 Bar</t>
-        </is>
-      </c>
-    </row>
-    <row r="53">
-      <c r="E53" t="inlineStr">
-        <is>
-          <t>Pad Plate</t>
-        </is>
-      </c>
-      <c r="G53" t="inlineStr">
-        <is>
-          <t>HOT WATER</t>
-        </is>
-      </c>
-      <c r="H53" t="inlineStr">
-        <is>
-          <t>Not Found</t>
-        </is>
-      </c>
-      <c r="I53" t="inlineStr">
-        <is>
-          <t>ASTM A36</t>
-        </is>
-      </c>
-      <c r="J53" t="inlineStr">
-        <is>
-          <t>A36</t>
-        </is>
-      </c>
-      <c r="K53" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-      <c r="L53" t="inlineStr">
-        <is>
-          <t>120 °C</t>
-        </is>
-      </c>
-      <c r="M53" t="inlineStr">
-        <is>
-          <t>4 Bar</t>
-        </is>
-      </c>
-      <c r="N53" t="inlineStr">
-        <is>
-          <t>90 °C</t>
-        </is>
-      </c>
-      <c r="O53" t="inlineStr">
-        <is>
-          <t>1 Bar</t>
+          <t>1 Bar G</t>
         </is>
       </c>
     </row>
@@ -3273,20 +3098,20 @@
   <mergeCells count="19">
     <mergeCell ref="D5:D7"/>
     <mergeCell ref="B3:B4"/>
+    <mergeCell ref="B8:B51"/>
     <mergeCell ref="H5:J6"/>
     <mergeCell ref="A5:A7"/>
     <mergeCell ref="G5:G7"/>
     <mergeCell ref="B5:B7"/>
-    <mergeCell ref="B8:B53"/>
     <mergeCell ref="A3:A4"/>
     <mergeCell ref="D3:D4"/>
-    <mergeCell ref="A8:A53"/>
-    <mergeCell ref="C8:C53"/>
+    <mergeCell ref="A8:A51"/>
+    <mergeCell ref="C8:C51"/>
+    <mergeCell ref="D8:D51"/>
     <mergeCell ref="C5:C7"/>
     <mergeCell ref="E5:E7"/>
     <mergeCell ref="K5:K7"/>
     <mergeCell ref="F5:F7"/>
-    <mergeCell ref="D8:D53"/>
     <mergeCell ref="C3:C4"/>
     <mergeCell ref="L5:M6"/>
     <mergeCell ref="N5:O6"/>

</xml_diff>